<commit_message>
Add a geolocation page
</commit_message>
<xml_diff>
--- a/bug-tracker.xlsx
+++ b/bug-tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>STATUS</t>
   </si>
@@ -42,15 +42,9 @@
     <t>Tuesday, April 20 ,2021</t>
   </si>
   <si>
-    <t>fix</t>
-  </si>
-  <si>
     <t>Webnesday, April 20, 2021</t>
   </si>
   <si>
-    <t>Allow db to store extra values in add couse form</t>
-  </si>
-  <si>
     <t>bug</t>
   </si>
   <si>
@@ -73,6 +67,45 @@
   </si>
   <si>
     <t>33ade9da13a327fdad44a3412c9e17bd08d1a58f</t>
+  </si>
+  <si>
+    <t>Resolve check box data redundancy in add course form</t>
+  </si>
+  <si>
+    <t>Improve location accuracy in geolocation</t>
+  </si>
+  <si>
+    <t>Fix error"setCenter: not a LatLng or LatLngLiteral with finite coordinates"</t>
+  </si>
+  <si>
+    <t>Thursday, April 20, 2021</t>
+  </si>
+  <si>
+    <t>unmet dependency</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>Db</t>
+  </si>
+  <si>
+    <t>Addform</t>
+  </si>
+  <si>
+    <t>Home/Home</t>
+  </si>
+  <si>
+    <t>Allow db to store extra values from add couse form</t>
+  </si>
+  <si>
+    <t>Addcourseform</t>
+  </si>
+  <si>
+    <t>Geolocation</t>
+  </si>
+  <si>
+    <t>Course</t>
   </si>
 </sst>
 </file>
@@ -151,6 +184,109 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3438525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9877425" y="1095375"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3286125</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="733425" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9725025" y="933450"/>
+          <a:ext cx="733425" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,21 +576,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="44.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="57.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -462,80 +599,147 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
-        <v>14</v>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix bugtracker to git ignore
</commit_message>
<xml_diff>
--- a/bug-tracker.xlsx
+++ b/bug-tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>STATUS</t>
   </si>
@@ -106,12 +106,21 @@
   </si>
   <si>
     <t>Course</t>
+  </si>
+  <si>
+    <t>course/actionCard</t>
+  </si>
+  <si>
+    <t>show action card only when its class time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,12 +168,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,6 +744,24 @@
       </c>
       <c r="F8" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5">
+        <f ca="1">TODAY()</f>
+        <v>44312</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix add bug tracker to git ignore
</commit_message>
<xml_diff>
--- a/bug-tracker.xlsx
+++ b/bug-tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>STATUS</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>show action card only when its class time</t>
+  </si>
+  <si>
+    <t>545e905dcec09f579fb05c55beab5bf79537641a</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -130,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +158,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -168,13 +177,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +600,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,8 +761,11 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
+      <c r="B9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D9" s="5">
         <f ca="1">TODAY()</f>

</xml_diff>